<commit_message>
Add PID and Scrum Board
</commit_message>
<xml_diff>
--- a/Scrum_Board.xlsx
+++ b/Scrum_Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-220" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,128 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>DOING</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TASK DESCRIPTION </t>
+  </si>
+  <si>
+    <t>OWNER</t>
+  </si>
+  <si>
+    <t>HOURS</t>
+  </si>
+  <si>
+    <t>Led Blink Pi 2</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Hardware ordering</t>
+  </si>
+  <si>
+    <t>Bart</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Documentation PID</t>
+  </si>
+  <si>
+    <t>Robbert</t>
+  </si>
+  <si>
+    <t>Robbert/Dennis</t>
+  </si>
+  <si>
+    <t>Scrum initalizing</t>
+  </si>
+  <si>
+    <t>Install buildroot</t>
+  </si>
+  <si>
+    <t>Git initalizing</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -28,13 +147,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,18 +192,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G23" totalsRowShown="0">
+  <autoFilter ref="A1:G23"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="PRIORITY"/>
+    <tableColumn id="2" name="TASK DESCRIPTION "/>
+    <tableColumn id="3" name="OWNER"/>
+    <tableColumn id="4" name="TODO"/>
+    <tableColumn id="5" name="DOING"/>
+    <tableColumn id="6" name="DONE"/>
+    <tableColumn id="7" name="HOURS" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,13 +553,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
scrum update sprint 3
</commit_message>
<xml_diff>
--- a/Scrum_Board.xlsx
+++ b/Scrum_Board.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\BeerTender\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>PRIORITY</t>
   </si>
@@ -143,16 +151,40 @@
   </si>
   <si>
     <t>3.7</t>
+  </si>
+  <si>
+    <t>cross compile module for pi</t>
+  </si>
+  <si>
+    <t>blink led module for pi</t>
+  </si>
+  <si>
+    <t>porting PWM naar pi2</t>
+  </si>
+  <si>
+    <t>algoritme besturing</t>
+  </si>
+  <si>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t>Dennis/Robbert</t>
+  </si>
+  <si>
+    <t>Jeroen</t>
+  </si>
+  <si>
+    <t>software architectuur</t>
+  </si>
+  <si>
+    <t>Dennis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -161,20 +193,10 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="9"/>
       <name val="Calibri"/>
@@ -183,6 +205,19 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -420,122 +455,130 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff4f81bd"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffb8cce4"/>
-      <rgbColor rgb="ffdbe5f1"/>
-      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFB8CCE4"/>
+      <rgbColor rgb="FFDBE5F1"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -727,7 +770,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -736,7 +779,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -745,7 +788,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -754,7 +797,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -763,7 +806,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -772,7 +815,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -884,8 +927,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -893,14 +936,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -919,7 +962,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +970,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -955,7 +998,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,7 +1024,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1007,7 +1050,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1076,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,7 +1102,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,7 +1128,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1111,7 +1154,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1137,7 +1180,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1163,7 +1206,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1176,9 +1219,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1194,7 +1243,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1213,7 +1262,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1288,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1314,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1340,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1366,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1392,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1369,7 +1418,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1395,7 +1444,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1421,7 +1470,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1447,7 +1496,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1460,9 +1509,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1475,7 +1530,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1494,7 +1549,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1524,7 +1579,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1550,7 +1605,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1576,7 +1631,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1602,7 +1657,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1628,7 +1683,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1654,7 +1709,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1680,7 +1735,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1706,7 +1761,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1732,7 +1787,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1745,169 +1800,176 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.125" style="1" customWidth="1"/>
-    <col min="9" max="256" width="8.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" style="1" customWidth="1"/>
+    <col min="4" max="256" width="8.09765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="4">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" ht="20" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="F2" t="s" s="7">
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" ht="19" customHeight="1">
-      <c r="A3" t="s" s="10">
+    <row r="3" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s" s="11">
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" t="s" s="11">
+      <c r="F3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" ht="19" customHeight="1">
-      <c r="A4" t="s" s="14">
+    <row r="4" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s" s="15">
+      <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s" s="15">
+      <c r="C4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
-      <c r="F4" t="s" s="15">
+      <c r="F4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" ht="19" customHeight="1">
-      <c r="A5" t="s" s="10">
+    <row r="5" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" t="s" s="11">
+      <c r="F5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" ht="19" customHeight="1">
-      <c r="A6" t="s" s="14">
+    <row r="6" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s" s="15">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s" s="15">
+      <c r="C6" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
-      <c r="F6" t="s" s="15">
+      <c r="F6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" ht="19" customHeight="1">
-      <c r="A7" t="s" s="10">
+    <row r="7" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="11">
+      <c r="C7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
-      <c r="F7" t="s" s="11">
+      <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="5"/>
+      <c r="I7" s="27" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="8" ht="19" customHeight="1">
-      <c r="A8" t="s" s="18">
+    <row r="8" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="19"/>
@@ -1917,99 +1979,102 @@
       <c r="F8" s="19"/>
       <c r="G8" s="20"/>
       <c r="H8" s="5"/>
+      <c r="I8" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="9" ht="19" customHeight="1">
-      <c r="A9" t="s" s="10">
+    <row r="9" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s" s="11">
+      <c r="B9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s" s="11">
+      <c r="C9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" t="s" s="11">
+      <c r="E9" s="11"/>
+      <c r="F9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="12"/>
       <c r="G9" s="13"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" ht="19" customHeight="1">
-      <c r="A10" t="s" s="14">
+    <row r="10" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s" s="15">
+      <c r="B10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s" s="15">
+      <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="16"/>
-      <c r="E10" t="s" s="15">
+      <c r="E10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" ht="19" customHeight="1">
-      <c r="A11" t="s" s="10">
+    <row r="11" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s" s="11">
+      <c r="B11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s" s="11">
+      <c r="C11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" t="s" s="11">
+      <c r="D11" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" ht="19" customHeight="1">
-      <c r="A12" t="s" s="14">
+    <row r="12" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s" s="15">
+      <c r="B12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s" s="15">
+      <c r="C12" s="15" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="16"/>
-      <c r="E12" t="s" s="15">
+      <c r="E12" s="15"/>
+      <c r="F12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="16"/>
       <c r="G12" s="17"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" ht="19" customHeight="1">
-      <c r="A13" t="s" s="10">
+    <row r="13" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s" s="11">
+      <c r="B13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C13" s="11" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" t="s" s="11">
+      <c r="E13" s="11"/>
+      <c r="F13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="12"/>
       <c r="G13" s="13"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" ht="19" customHeight="1">
-      <c r="A14" t="s" s="18">
+    <row r="14" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="19"/>
@@ -2020,68 +2085,98 @@
       <c r="G14" s="20"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" ht="19" customHeight="1">
-      <c r="A15" t="s" s="14">
+    <row r="15" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" ht="19" customHeight="1">
-      <c r="A16" t="s" s="10">
+    <row r="16" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="13"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" ht="19" customHeight="1">
-      <c r="A17" t="s" s="14">
+    <row r="17" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" ht="19" customHeight="1">
-      <c r="A18" t="s" s="10">
+    <row r="18" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="B18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>10</v>
+      </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="13"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" ht="19" customHeight="1">
-      <c r="A19" t="s" s="14">
+    <row r="19" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" ht="19" customHeight="1">
-      <c r="A20" t="s" s="10">
+    <row r="20" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="12"/>
@@ -2092,8 +2187,8 @@
       <c r="G20" s="13"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" ht="19" customHeight="1">
-      <c r="A21" t="s" s="14">
+    <row r="21" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="16"/>
@@ -2104,7 +2199,7 @@
       <c r="G21" s="17"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" ht="19" customHeight="1">
+    <row r="22" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
@@ -2114,7 +2209,7 @@
       <c r="G22" s="23"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" ht="19" customHeight="1">
+    <row r="23" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
@@ -2126,7 +2221,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>